<commit_message>
Make Elite Enemy and Deffault Enemy modify
</commit_message>
<xml_diff>
--- a/Client/Resources/Data/Animation/Enemy/Elite/EliteEnemy.xlsx
+++ b/Client/Resources/Data/Animation/Enemy/Elite/EliteEnemy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ArcheTypeZero\GA_6th_2Q_Project\Client\Resources\Data\Animation\Enemy\Elite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A225003F-9849-4BFC-ACE7-AF6C61169954}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B1E503-B7DB-4D06-9281-F4035DFD1A27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Animation</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,7 +59,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Enemy_Elite_Attack</t>
+    <t>Enemy_Elite_SwordSwing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy_Elite_SwordStab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy_Elite_Up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Death</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy_Elite_Death</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -385,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -407,7 +431,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>COUNTA(A3:A39)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -440,6 +464,39 @@
         <v>8</v>
       </c>
       <c r="C5">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
         <v>0.06</v>
       </c>
     </row>

</xml_diff>